<commit_message>
move some ship related function in the ga.py to the ship.py
</commit_message>
<xml_diff>
--- a/output/full_rule.xlsx
+++ b/output/full_rule.xlsx
@@ -371,7 +371,7 @@
   <dimension ref="A1:A180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -407,21 +407,21 @@
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -435,7 +435,7 @@
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -967,14 +967,14 @@
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1037,14 +1037,14 @@
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1065,21 +1065,21 @@
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1135,7 +1135,7 @@
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1408,7 +1408,7 @@
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1562,7 +1562,7 @@
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1576,7 +1576,7 @@
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add set function and comment out
</commit_message>
<xml_diff>
--- a/output/full_rule.xlsx
+++ b/output/full_rule.xlsx
@@ -400,7 +400,7 @@
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -526,14 +526,14 @@
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -554,14 +554,14 @@
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -841,14 +841,14 @@
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1205,7 +1205,7 @@
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1303,21 +1303,21 @@
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1331,14 +1331,14 @@
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1352,7 +1352,7 @@
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1373,7 +1373,7 @@
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1597,7 +1597,7 @@
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify adapt_rule function. According to it, modify fitness_function also.
</commit_message>
<xml_diff>
--- a/output/full_rule.xlsx
+++ b/output/full_rule.xlsx
@@ -855,7 +855,7 @@
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1016,14 +1016,14 @@
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1163,14 +1163,14 @@
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify rule_adpate, crossing and mutation
</commit_message>
<xml_diff>
--- a/output/full_rule.xlsx
+++ b/output/full_rule.xlsx
@@ -561,14 +561,14 @@
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -946,42 +946,42 @@
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1170,21 +1170,21 @@
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Store the best individual unchanged
</commit_message>
<xml_diff>
--- a/output/full_rule.xlsx
+++ b/output/full_rule.xlsx
@@ -813,14 +813,14 @@
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -953,21 +953,21 @@
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -988,14 +988,14 @@
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>STAY</t>
+          <t>CHARTER</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
@@ -1170,21 +1170,21 @@
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>CHARTER</t>
+          <t>STAY</t>
         </is>
       </c>
     </row>

</xml_diff>